<commit_message>
More "previously unexpressing" models from Claire. Try using these to validate models generated on 2016-05-11 data.
</commit_message>
<xml_diff>
--- a/2016-06-16/props.xlsx
+++ b/2016-06-16/props.xlsx
@@ -19,10 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
-  <si>
-    <t>chimera</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>mKate_pix</t>
   </si>
@@ -63,21 +60,12 @@
     <t>sum_ratio</t>
   </si>
   <si>
-    <t>CsChrim</t>
-  </si>
-  <si>
-    <t>C1C2</t>
-  </si>
-  <si>
     <t>CheRiff</t>
   </si>
   <si>
     <t>c12</t>
   </si>
   <si>
-    <t>c17</t>
-  </si>
-  <si>
     <t>c18</t>
   </si>
   <si>
@@ -129,9 +117,6 @@
     <t>n31</t>
   </si>
   <si>
-    <t>n33</t>
-  </si>
-  <si>
     <t>n54</t>
   </si>
   <si>
@@ -163,6 +148,15 @@
   </si>
   <si>
     <t>CsCbChR1</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>cschrimson</t>
+  </si>
+  <si>
+    <t>c1c2</t>
   </si>
 </sst>
 </file>
@@ -532,59 +526,61 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N35"/>
+  <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
-      </c>
-      <c r="N1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
       <c r="B2">
         <v>0.98891579255899997</v>
@@ -628,7 +624,7 @@
     </row>
     <row r="3" spans="1:14">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="B3">
         <v>0.96690323758899999</v>
@@ -672,7 +668,7 @@
     </row>
     <row r="4" spans="1:14">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B4">
         <v>0.30911307622400003</v>
@@ -716,7 +712,7 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B5">
         <v>1.10933175549</v>
@@ -760,1243 +756,1233 @@
     </row>
     <row r="6" spans="1:14">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>15</v>
+      </c>
+      <c r="B6">
+        <v>0.40057696125100001</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>4.0001415983599999E-2</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>1.7926374007799999</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>5.68076057954E-2</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0.103300286688</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>3.14903657677E-2</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>5.86824196471E-3</v>
       </c>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B7">
-        <v>0.40057696125100001</v>
+        <v>0.60018260273000001</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>0.123799427884</v>
       </c>
       <c r="D7">
-        <v>4.0001415983599999E-2</v>
+        <v>2.4130624715899999E-2</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>8.23703869545E-3</v>
       </c>
       <c r="F7">
-        <v>1.7926374007799999</v>
+        <v>0.52753918469299999</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>0.15652604784800001</v>
       </c>
       <c r="H7">
-        <v>5.68076057954E-2</v>
+        <v>4.8750170860100001E-2</v>
       </c>
       <c r="I7">
-        <v>0</v>
+        <v>1.9309131865399998E-2</v>
       </c>
       <c r="J7">
-        <v>0.103300286688</v>
+        <v>3.9714370193200003E-2</v>
       </c>
       <c r="K7">
-        <v>0</v>
+        <v>6.8472794333500004E-3</v>
       </c>
       <c r="L7">
-        <v>3.14903657677E-2</v>
+        <v>9.8563122885800006E-2</v>
       </c>
       <c r="M7">
-        <v>0</v>
+        <v>3.5820089806000002E-2</v>
       </c>
       <c r="N7">
-        <v>5.86824196471E-3</v>
+        <v>1.9470630410499999E-3</v>
       </c>
     </row>
     <row r="8" spans="1:14">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B8">
-        <v>0.60018260273000001</v>
+        <v>0.331948257079</v>
       </c>
       <c r="C8">
-        <v>0.123799427884</v>
+        <v>8.1220305839300002E-4</v>
       </c>
       <c r="D8">
-        <v>2.4130624715899999E-2</v>
+        <v>4.1740656573600002E-2</v>
       </c>
       <c r="E8">
-        <v>8.23703869545E-3</v>
+        <v>1.02721315053E-2</v>
       </c>
       <c r="F8">
-        <v>0.52753918469299999</v>
+        <v>0.771474919446</v>
       </c>
       <c r="G8">
-        <v>0.15652604784800001</v>
+        <v>0.40286389907199999</v>
       </c>
       <c r="H8">
-        <v>4.8750170860100001E-2</v>
+        <v>0.15815956437299999</v>
       </c>
       <c r="I8">
-        <v>1.9309131865399998E-2</v>
+        <v>4.48096490108E-2</v>
       </c>
       <c r="J8">
-        <v>3.9714370193200003E-2</v>
+        <v>0.12369722029999999</v>
       </c>
       <c r="K8">
-        <v>6.8472794333500004E-3</v>
+        <v>2.7699316032000001E-2</v>
       </c>
       <c r="L8">
-        <v>9.8563122885800006E-2</v>
+        <v>0.33130653185699999</v>
       </c>
       <c r="M8">
-        <v>3.5820089806000002E-2</v>
+        <v>0.21212956242799999</v>
       </c>
       <c r="N8">
-        <v>1.9470630410499999E-3</v>
+        <v>1.8322701847700001E-2</v>
       </c>
     </row>
     <row r="9" spans="1:14">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B9">
-        <v>0.331948257079</v>
+        <v>1.1741329061300001</v>
       </c>
       <c r="C9">
-        <v>8.1220305839300002E-4</v>
+        <v>0.43534755004999998</v>
       </c>
       <c r="D9">
-        <v>4.1740656573600002E-2</v>
+        <v>0.112989642214</v>
       </c>
       <c r="E9">
-        <v>1.02721315053E-2</v>
+        <v>5.3203069677400003E-2</v>
       </c>
       <c r="F9">
-        <v>0.771474919446</v>
+        <v>2.41417333363</v>
       </c>
       <c r="G9">
-        <v>0.40286389907199999</v>
+        <v>0.77297583880599996</v>
       </c>
       <c r="H9">
-        <v>0.15815956437299999</v>
+        <v>7.0387964867600003E-2</v>
       </c>
       <c r="I9">
-        <v>4.48096490108E-2</v>
+        <v>1.7299976747800001E-2</v>
       </c>
       <c r="J9">
-        <v>0.12369722029999999</v>
+        <v>9.2580499992099996E-2</v>
       </c>
       <c r="K9">
-        <v>2.7699316032000001E-2</v>
+        <v>2.0794961664200001E-2</v>
       </c>
       <c r="L9">
-        <v>0.33130653185699999</v>
+        <v>3.08748985298E-2</v>
       </c>
       <c r="M9">
-        <v>0.21212956242799999</v>
+        <v>3.8288913201999998E-3</v>
       </c>
       <c r="N9">
-        <v>1.8322701847700001E-2</v>
+        <v>6.8694527747699997E-3</v>
       </c>
     </row>
     <row r="10" spans="1:14">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B10">
-        <v>1.1741329061300001</v>
+        <v>0.86743376917299997</v>
       </c>
       <c r="C10">
-        <v>0.43534755004999998</v>
+        <v>0.22358709780200001</v>
       </c>
       <c r="D10">
-        <v>0.112989642214</v>
+        <v>0.12620551921199999</v>
       </c>
       <c r="E10">
-        <v>5.3203069677400003E-2</v>
+        <v>5.5024929852199998E-2</v>
       </c>
       <c r="F10">
-        <v>2.41417333363</v>
+        <v>0.32027999469099999</v>
       </c>
       <c r="G10">
-        <v>0.77297583880599996</v>
+        <v>3.1581925227199999E-2</v>
       </c>
       <c r="H10">
-        <v>7.0387964867600003E-2</v>
+        <v>0.128103092763</v>
       </c>
       <c r="I10">
-        <v>1.7299976747800001E-2</v>
+        <v>2.8442665886100001E-2</v>
       </c>
       <c r="J10">
-        <v>9.2580499992099996E-2</v>
+        <v>0.136665896107</v>
       </c>
       <c r="K10">
-        <v>2.0794961664200001E-2</v>
+        <v>3.1829712913500001E-2</v>
       </c>
       <c r="L10">
-        <v>3.08748985298E-2</v>
+        <v>0.41163054420400003</v>
       </c>
       <c r="M10">
-        <v>3.8288913201999998E-3</v>
+        <v>0.10739243687900001</v>
       </c>
       <c r="N10">
-        <v>6.8694527747699997E-3</v>
+        <v>1.7083977372799999E-2</v>
       </c>
     </row>
     <row r="11" spans="1:14">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B11">
-        <v>0.86743376917299997</v>
+        <v>0.78751069397200002</v>
       </c>
       <c r="C11">
-        <v>0.22358709780200001</v>
+        <v>0.36934016667899999</v>
       </c>
       <c r="D11">
-        <v>0.12620551921199999</v>
+        <v>9.3725013588000006E-2</v>
       </c>
       <c r="E11">
-        <v>5.5024929852199998E-2</v>
+        <v>7.4917276165499994E-2</v>
       </c>
       <c r="F11">
-        <v>0.32027999469099999</v>
+        <v>2.1896439703500001</v>
       </c>
       <c r="G11">
-        <v>3.1581925227199999E-2</v>
+        <v>1.11616034075</v>
       </c>
       <c r="H11">
-        <v>0.128103092763</v>
+        <v>5.7054001292999999E-2</v>
       </c>
       <c r="I11">
-        <v>2.8442665886100001E-2</v>
+        <v>1.9675918078599999E-2</v>
       </c>
       <c r="J11">
-        <v>0.136665896107</v>
+        <v>9.7211866763199997E-2</v>
       </c>
       <c r="K11">
-        <v>3.1829712913500001E-2</v>
+        <v>4.7118390439900001E-2</v>
       </c>
       <c r="L11">
-        <v>0.41163054420400003</v>
+        <v>3.7201358777200003E-2</v>
       </c>
       <c r="M11">
-        <v>0.10739243687900001</v>
+        <v>3.7560190690299998E-2</v>
       </c>
       <c r="N11">
-        <v>1.7083977372799999E-2</v>
+        <v>6.03312549749E-3</v>
       </c>
     </row>
     <row r="12" spans="1:14">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B12">
-        <v>0.78751069397200002</v>
+        <v>0.27703846285</v>
       </c>
       <c r="C12">
-        <v>0.36934016667899999</v>
+        <v>4.70746310923E-2</v>
       </c>
       <c r="D12">
-        <v>9.3725013588000006E-2</v>
+        <v>2.95554166385E-2</v>
       </c>
       <c r="E12">
-        <v>7.4917276165499994E-2</v>
+        <v>7.46002468878E-3</v>
       </c>
       <c r="F12">
-        <v>2.1896439703500001</v>
+        <v>0.29986516354199999</v>
       </c>
       <c r="G12">
-        <v>1.11616034075</v>
+        <v>3.5747678613099999E-2</v>
       </c>
       <c r="H12">
-        <v>5.7054001292999999E-2</v>
+        <v>0.110034266844</v>
       </c>
       <c r="I12">
-        <v>1.9675918078599999E-2</v>
+        <v>5.7621410263099998E-2</v>
       </c>
       <c r="J12">
-        <v>9.7211866763199997E-2</v>
+        <v>0.114334206427</v>
       </c>
       <c r="K12">
-        <v>4.7118390439900001E-2</v>
+        <v>3.9851725087899997E-2</v>
       </c>
       <c r="L12">
-        <v>3.7201358777200003E-2</v>
+        <v>0.39659362839700002</v>
       </c>
       <c r="M12">
-        <v>3.7560190690299998E-2</v>
+        <v>0.206821804704</v>
       </c>
       <c r="N12">
-        <v>6.03312549749E-3</v>
+        <v>1.4453100314099999E-2</v>
       </c>
     </row>
     <row r="13" spans="1:14">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B13">
-        <v>0.27703846285</v>
+        <v>0.193016657732</v>
       </c>
       <c r="C13">
-        <v>4.70746310923E-2</v>
+        <v>5.9174576543199998E-2</v>
       </c>
       <c r="D13">
-        <v>2.95554166385E-2</v>
+        <v>6.0012878155800004E-3</v>
       </c>
       <c r="E13">
-        <v>7.46002468878E-3</v>
+        <v>3.9602297378499999E-3</v>
       </c>
       <c r="F13">
-        <v>0.29986516354199999</v>
+        <v>0.23007778830200001</v>
       </c>
       <c r="G13">
-        <v>3.5747678613099999E-2</v>
+        <v>3.47706563139E-2</v>
       </c>
       <c r="H13">
-        <v>0.110034266844</v>
+        <v>7.4526474374599999E-2</v>
       </c>
       <c r="I13">
-        <v>5.7621410263099998E-2</v>
+        <v>9.0172290938900002E-2</v>
       </c>
       <c r="J13">
-        <v>0.114334206427</v>
+        <v>3.4204999354899998E-2</v>
       </c>
       <c r="K13">
-        <v>3.9851725087899997E-2</v>
+        <v>1.8191309620900001E-2</v>
       </c>
       <c r="L13">
-        <v>0.39659362839700002</v>
+        <v>0.27809742133400001</v>
       </c>
       <c r="M13">
-        <v>0.206821804704</v>
+        <v>0.29596795372399998</v>
       </c>
       <c r="N13">
-        <v>1.4453100314099999E-2</v>
+        <v>4.1271426564999996E-3</v>
       </c>
     </row>
     <row r="14" spans="1:14">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B14">
-        <v>0.193016657732</v>
+        <v>0.91559488449799997</v>
       </c>
       <c r="C14">
-        <v>5.9174576543199998E-2</v>
+        <v>0.15747565146699999</v>
       </c>
       <c r="D14">
-        <v>6.0012878155800004E-3</v>
+        <v>1.1888282338299999E-2</v>
       </c>
       <c r="E14">
-        <v>3.9602297378499999E-3</v>
+        <v>4.65340431904E-3</v>
       </c>
       <c r="F14">
-        <v>0.23007778830200001</v>
+        <v>0.57696677311099998</v>
       </c>
       <c r="G14">
-        <v>3.47706563139E-2</v>
+        <v>4.5538213740999998E-2</v>
       </c>
       <c r="H14">
-        <v>7.4526474374599999E-2</v>
+        <v>1.8725065223599999E-2</v>
       </c>
       <c r="I14">
-        <v>9.0172290938900002E-2</v>
+        <v>3.1856410677E-3</v>
       </c>
       <c r="J14">
-        <v>3.4204999354899998E-2</v>
+        <v>1.29335778519E-2</v>
       </c>
       <c r="K14">
-        <v>1.8191309620900001E-2</v>
+        <v>3.2669077030200002E-3</v>
       </c>
       <c r="L14">
-        <v>0.27809742133400001</v>
+        <v>3.2319053732400002E-2</v>
       </c>
       <c r="M14">
-        <v>0.29596795372399998</v>
+        <v>3.67306525472E-3</v>
       </c>
       <c r="N14">
-        <v>4.1271426564999996E-3</v>
+        <v>2.5204601284700001E-4</v>
       </c>
     </row>
     <row r="15" spans="1:14">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B15">
-        <v>0.91559488449799997</v>
+        <v>0.27497912885499998</v>
       </c>
       <c r="C15">
-        <v>0.15747565146699999</v>
+        <v>6.9659467792400004E-3</v>
       </c>
       <c r="D15">
-        <v>1.1888282338299999E-2</v>
+        <v>2.8991711572799998E-2</v>
       </c>
       <c r="E15">
-        <v>4.65340431904E-3</v>
+        <v>1.5130395011200001E-2</v>
       </c>
       <c r="F15">
-        <v>0.57696677311099998</v>
+        <v>0.23952440122099999</v>
       </c>
       <c r="G15">
-        <v>4.5538213740999998E-2</v>
+        <v>5.6426836164899997E-2</v>
       </c>
       <c r="H15">
-        <v>1.8725065223599999E-2</v>
+        <v>8.5008645544099995E-2</v>
       </c>
       <c r="I15">
-        <v>3.1856410677E-3</v>
+        <v>4.3024270931099999E-2</v>
       </c>
       <c r="J15">
-        <v>1.29335778519E-2</v>
+        <v>0.104613934071</v>
       </c>
       <c r="K15">
-        <v>3.2669077030200002E-3</v>
+        <v>5.4645752668400001E-2</v>
       </c>
       <c r="L15">
-        <v>3.2319053732400002E-2</v>
+        <v>0.41458026697900002</v>
       </c>
       <c r="M15">
-        <v>3.67306525472E-3</v>
+        <v>0.27126677983199998</v>
       </c>
       <c r="N15">
-        <v>2.5204601284700001E-4</v>
+        <v>1.1244182508399999E-2</v>
       </c>
     </row>
     <row r="16" spans="1:14">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B16">
-        <v>0.27497912885499998</v>
+        <v>0.58061004600199995</v>
       </c>
       <c r="C16">
-        <v>6.9659467792400004E-3</v>
+        <v>0.144519941018</v>
       </c>
       <c r="D16">
-        <v>2.8991711572799998E-2</v>
+        <v>6.05583134989E-2</v>
       </c>
       <c r="E16">
-        <v>1.5130395011200001E-2</v>
+        <v>1.8380645179799999E-2</v>
       </c>
       <c r="F16">
-        <v>0.23952440122099999</v>
+        <v>0.68311859108899997</v>
       </c>
       <c r="G16">
-        <v>5.6426836164899997E-2</v>
+        <v>0.25673533064699999</v>
       </c>
       <c r="H16">
-        <v>8.5008645544099995E-2</v>
+        <v>0.115334733105</v>
       </c>
       <c r="I16">
-        <v>4.3024270931099999E-2</v>
+        <v>5.1533850594299997E-2</v>
       </c>
       <c r="J16">
-        <v>0.104613934071</v>
+        <v>0.10535184847</v>
       </c>
       <c r="K16">
-        <v>5.4645752668400001E-2</v>
+        <v>1.42972365657E-2</v>
       </c>
       <c r="L16">
-        <v>0.41458026697900002</v>
+        <v>0.16452092205900001</v>
       </c>
       <c r="M16">
-        <v>0.27126677983199998</v>
+        <v>1.4607912725900001E-2</v>
       </c>
       <c r="N16">
-        <v>1.1244182508399999E-2</v>
+        <v>1.14177743395E-2</v>
       </c>
     </row>
     <row r="17" spans="1:14">
       <c r="A17" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B17">
-        <v>0.58061004600199995</v>
+        <v>0.80289928604399996</v>
       </c>
       <c r="C17">
-        <v>0.144519941018</v>
+        <v>0.168270756976</v>
       </c>
       <c r="D17">
-        <v>6.05583134989E-2</v>
+        <v>9.0180629407500004E-2</v>
       </c>
       <c r="E17">
-        <v>1.8380645179799999E-2</v>
+        <v>3.7500245244600001E-2</v>
       </c>
       <c r="F17">
-        <v>0.68311859108899997</v>
+        <v>2.0710708595899998</v>
       </c>
       <c r="G17">
-        <v>0.25673533064699999</v>
+        <v>0.44509626095799998</v>
       </c>
       <c r="H17">
-        <v>0.115334733105</v>
+        <v>7.0309138527099996E-2</v>
       </c>
       <c r="I17">
-        <v>5.1533850594299997E-2</v>
+        <v>1.7534925912599999E-2</v>
       </c>
       <c r="J17">
-        <v>0.10535184847</v>
+        <v>0.108835118109</v>
       </c>
       <c r="K17">
-        <v>1.42972365657E-2</v>
+        <v>4.0676062874800002E-2</v>
       </c>
       <c r="L17">
-        <v>0.16452092205900001</v>
+        <v>3.4750962613899997E-2</v>
       </c>
       <c r="M17">
-        <v>1.4607912725900001E-2</v>
+        <v>7.4819779157800003E-3</v>
       </c>
       <c r="N17">
-        <v>1.14177743395E-2</v>
+        <v>8.2691570672899992E-3</v>
       </c>
     </row>
     <row r="18" spans="1:14">
       <c r="A18" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B18">
-        <v>0.80289928604399996</v>
+        <v>0.50273172961500001</v>
       </c>
       <c r="C18">
-        <v>0.168270756976</v>
+        <v>0.11365952087800001</v>
       </c>
       <c r="D18">
-        <v>9.0180629407500004E-2</v>
+        <v>1.9493478989100001E-2</v>
       </c>
       <c r="E18">
-        <v>3.7500245244600001E-2</v>
+        <v>7.1720953023E-3</v>
       </c>
       <c r="F18">
-        <v>2.0710708595899998</v>
+        <v>0.17735624608600001</v>
       </c>
       <c r="G18">
-        <v>0.44509626095799998</v>
+        <v>2.1895792161199999E-2</v>
       </c>
       <c r="H18">
-        <v>7.0309138527099996E-2</v>
+        <v>4.4975569615299998E-2</v>
       </c>
       <c r="I18">
-        <v>1.7534925912599999E-2</v>
+        <v>9.1411235906000005E-3</v>
       </c>
       <c r="J18">
-        <v>0.108835118109</v>
+        <v>3.8196614891100003E-2</v>
       </c>
       <c r="K18">
-        <v>4.0676062874800002E-2</v>
+        <v>9.1962668463000004E-3</v>
       </c>
       <c r="L18">
-        <v>3.4750962613899997E-2</v>
+        <v>0.25764306125300002</v>
       </c>
       <c r="M18">
-        <v>7.4819779157800003E-3</v>
+        <v>4.3734260030399999E-2</v>
       </c>
       <c r="N18">
-        <v>8.2691570672899992E-3</v>
+        <v>1.7946582270599999E-3</v>
       </c>
     </row>
     <row r="19" spans="1:14">
       <c r="A19" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B19">
-        <v>0.50273172961500001</v>
+        <v>0.91311641457500003</v>
       </c>
       <c r="C19">
-        <v>0.11365952087800001</v>
+        <v>0.25170488772600003</v>
       </c>
       <c r="D19">
-        <v>1.9493478989100001E-2</v>
+        <v>9.2710819138799999E-2</v>
       </c>
       <c r="E19">
-        <v>7.1720953023E-3</v>
+        <v>3.9033716615500001E-2</v>
       </c>
       <c r="F19">
-        <v>0.17735624608600001</v>
+        <v>2.4976497343699999</v>
       </c>
       <c r="G19">
-        <v>2.1895792161199999E-2</v>
+        <v>0.34502222474900002</v>
       </c>
       <c r="H19">
-        <v>4.4975569615299998E-2</v>
+        <v>0.10062343281900001</v>
       </c>
       <c r="I19">
-        <v>9.1411235906000005E-3</v>
+        <v>4.6031358182999998E-2</v>
       </c>
       <c r="J19">
-        <v>3.8196614891100003E-2</v>
+        <v>9.7162162341500005E-2</v>
       </c>
       <c r="K19">
-        <v>9.1962668463000004E-3</v>
+        <v>1.9516919586399999E-2</v>
       </c>
       <c r="L19">
-        <v>0.25764306125300002</v>
+        <v>4.1434031632199997E-2</v>
       </c>
       <c r="M19">
-        <v>4.3734260030399999E-2</v>
+        <v>2.32758938818E-2</v>
       </c>
       <c r="N19">
-        <v>1.7946582270599999E-3</v>
+        <v>9.5277301213799997E-3</v>
       </c>
     </row>
     <row r="20" spans="1:14">
       <c r="A20" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B20">
-        <v>0.91311641457500003</v>
+        <v>0.179289614524</v>
       </c>
       <c r="C20">
-        <v>0.25170488772600003</v>
+        <v>9.0845166173300004E-2</v>
       </c>
       <c r="D20">
-        <v>9.2710819138799999E-2</v>
+        <v>1.0125271125800001E-2</v>
       </c>
       <c r="E20">
-        <v>3.9033716615500001E-2</v>
+        <v>8.8789860888200001E-3</v>
       </c>
       <c r="F20">
-        <v>2.4976497343699999</v>
+        <v>0.15218337321200001</v>
       </c>
       <c r="G20">
-        <v>0.34502222474900002</v>
+        <v>1.9479358174899999E-2</v>
       </c>
       <c r="H20">
-        <v>0.10062343281900001</v>
+        <v>7.5182088228800001E-2</v>
       </c>
       <c r="I20">
-        <v>4.6031358182999998E-2</v>
+        <v>7.9721530078200001E-2</v>
       </c>
       <c r="J20">
-        <v>9.7162162341500005E-2</v>
+        <v>4.9956030722700002E-2</v>
       </c>
       <c r="K20">
-        <v>1.9516919586399999E-2</v>
+        <v>2.0186435337999999E-2</v>
       </c>
       <c r="L20">
-        <v>4.1434031632199997E-2</v>
+        <v>0.43928685407000001</v>
       </c>
       <c r="M20">
-        <v>2.32758938818E-2</v>
+        <v>0.41773546837699999</v>
       </c>
       <c r="N20">
-        <v>9.5277301213799997E-3</v>
+        <v>5.3525471930200002E-3</v>
       </c>
     </row>
     <row r="21" spans="1:14">
       <c r="A21" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B21">
-        <v>0.179289614524</v>
+        <v>0.29750139978599999</v>
       </c>
       <c r="C21">
-        <v>9.0845166173300004E-2</v>
+        <v>6.7602271516699994E-2</v>
       </c>
       <c r="D21">
-        <v>1.0125271125800001E-2</v>
+        <v>1.0679031484499999E-2</v>
       </c>
       <c r="E21">
-        <v>8.8789860888200001E-3</v>
+        <v>3.32060171333E-3</v>
       </c>
       <c r="F21">
-        <v>0.15218337321200001</v>
+        <v>0.36732376037800002</v>
       </c>
       <c r="G21">
-        <v>1.9479358174899999E-2</v>
+        <v>3.61276579308E-2</v>
       </c>
       <c r="H21">
-        <v>7.5182088228800001E-2</v>
+        <v>4.4093541955800002E-2</v>
       </c>
       <c r="I21">
-        <v>7.9721530078200001E-2</v>
+        <v>5.69327284973E-3</v>
       </c>
       <c r="J21">
-        <v>4.9956030722700002E-2</v>
+        <v>3.87321791478E-2</v>
       </c>
       <c r="K21">
-        <v>2.0186435337999999E-2</v>
+        <v>5.0950753133999997E-3</v>
       </c>
       <c r="L21">
-        <v>0.43928685407000001</v>
+        <v>0.140363346552</v>
       </c>
       <c r="M21">
-        <v>0.41773546837699999</v>
+        <v>2.52960304099E-2</v>
       </c>
       <c r="N21">
-        <v>5.3525471930200002E-3</v>
+        <v>1.7295302405000001E-3</v>
       </c>
     </row>
     <row r="22" spans="1:14">
       <c r="A22" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B22">
-        <v>0.29750139978599999</v>
+        <v>0.25613148009699999</v>
       </c>
       <c r="C22">
-        <v>6.7602271516699994E-2</v>
+        <v>9.2798308762699996E-2</v>
       </c>
       <c r="D22">
-        <v>1.0679031484499999E-2</v>
+        <v>1.62092447773E-2</v>
       </c>
       <c r="E22">
-        <v>3.32060171333E-3</v>
+        <v>6.8332272575799997E-3</v>
       </c>
       <c r="F22">
-        <v>0.36732376037800002</v>
+        <v>0.38816538787799998</v>
       </c>
       <c r="G22">
-        <v>3.61276579308E-2</v>
+        <v>2.69813405503E-2</v>
       </c>
       <c r="H22">
-        <v>4.4093541955800002E-2</v>
+        <v>6.7333696948799995E-2</v>
       </c>
       <c r="I22">
-        <v>5.69327284973E-3</v>
+        <v>6.6197133090000002E-3</v>
       </c>
       <c r="J22">
-        <v>3.87321791478E-2</v>
+        <v>6.1544696795199999E-2</v>
       </c>
       <c r="K22">
-        <v>5.0950753133999997E-3</v>
+        <v>1.11015791041E-2</v>
       </c>
       <c r="L22">
-        <v>0.140363346552</v>
+        <v>0.18354633574400001</v>
       </c>
       <c r="M22">
-        <v>2.52960304099E-2</v>
+        <v>3.2565059469100002E-2</v>
       </c>
       <c r="N22">
-        <v>1.7295302405000001E-3</v>
+        <v>4.1790505966799998E-3</v>
       </c>
     </row>
     <row r="23" spans="1:14">
       <c r="A23" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B23">
-        <v>0.25613148009699999</v>
+        <v>0.67824824029200004</v>
       </c>
       <c r="C23">
-        <v>9.2798308762699996E-2</v>
+        <v>0.33829977076700002</v>
       </c>
       <c r="D23">
-        <v>1.62092447773E-2</v>
+        <v>0.42775674651899998</v>
       </c>
       <c r="E23">
-        <v>6.8332272575799997E-3</v>
+        <v>0.29715965308999998</v>
       </c>
       <c r="F23">
-        <v>0.38816538787799998</v>
+        <v>0.25193706911000002</v>
       </c>
       <c r="G23">
-        <v>2.69813405503E-2</v>
+        <v>2.29553848369E-2</v>
       </c>
       <c r="H23">
-        <v>6.7333696948799995E-2</v>
+        <v>0.168388528338</v>
       </c>
       <c r="I23">
-        <v>6.6197133090000002E-3</v>
+        <v>7.8004945187599997E-2</v>
       </c>
       <c r="J23">
-        <v>6.1544696795199999E-2</v>
+        <v>0.50164630941300004</v>
       </c>
       <c r="K23">
-        <v>1.11015791041E-2</v>
+        <v>0.25203821659499998</v>
       </c>
       <c r="L23">
-        <v>0.18354633574400001</v>
+        <v>0.68903048139</v>
       </c>
       <c r="M23">
-        <v>3.2565059469100002E-2</v>
+        <v>0.34790504848100001</v>
       </c>
       <c r="N23">
-        <v>4.1790505966799998E-3</v>
+        <v>0.10404213625399999</v>
       </c>
     </row>
     <row r="24" spans="1:14">
       <c r="A24" t="s">
-        <v>36</v>
+        <v>33</v>
+      </c>
+      <c r="B24">
+        <v>0.29781630003300003</v>
+      </c>
+      <c r="C24">
+        <v>4.0449302027199999E-2</v>
+      </c>
+      <c r="D24">
+        <v>1.5681822219E-2</v>
+      </c>
+      <c r="E24">
+        <v>4.2234778767100004E-3</v>
+      </c>
+      <c r="F24">
+        <v>0.37980985038699999</v>
+      </c>
+      <c r="G24">
+        <v>7.6775131166400001E-2</v>
+      </c>
+      <c r="H24">
+        <v>7.1728204485400002E-2</v>
+      </c>
+      <c r="I24">
+        <v>1.22806837352E-2</v>
+      </c>
+      <c r="J24">
+        <v>5.2453292880499998E-2</v>
+      </c>
+      <c r="K24">
+        <v>7.6377590244500002E-3</v>
+      </c>
+      <c r="L24">
+        <v>0.189595990435</v>
+      </c>
+      <c r="M24">
+        <v>3.2095626702099998E-2</v>
+      </c>
+      <c r="N24">
+        <v>3.8547348725099999E-3</v>
       </c>
     </row>
     <row r="25" spans="1:14">
       <c r="A25" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B25">
-        <v>0.67824824029200004</v>
+        <v>0.42154485009600001</v>
       </c>
       <c r="C25">
-        <v>0.33829977076700002</v>
+        <v>0.22025467257199999</v>
       </c>
       <c r="D25">
-        <v>0.42775674651899998</v>
+        <v>5.5069795328300003E-2</v>
       </c>
       <c r="E25">
-        <v>0.29715965308999998</v>
+        <v>4.2559313626299999E-2</v>
       </c>
       <c r="F25">
-        <v>0.25193706911000002</v>
+        <v>0.24085862439799999</v>
       </c>
       <c r="G25">
-        <v>2.29553848369E-2</v>
+        <v>3.92509252837E-2</v>
       </c>
       <c r="H25">
-        <v>0.168388528338</v>
+        <v>7.4110582985800005E-2</v>
       </c>
       <c r="I25">
-        <v>7.8004945187599997E-2</v>
+        <v>1.6007382192299999E-2</v>
       </c>
       <c r="J25">
-        <v>0.50164630941300004</v>
+        <v>0.111612573944</v>
       </c>
       <c r="K25">
-        <v>0.25203821659499998</v>
+        <v>3.6013227203299997E-2</v>
       </c>
       <c r="L25">
-        <v>0.68903048139</v>
+        <v>0.34027516914700001</v>
       </c>
       <c r="M25">
-        <v>0.34790504848100001</v>
+        <v>0.136348401614</v>
       </c>
       <c r="N25">
-        <v>0.10404213625399999</v>
+        <v>8.6278313539199999E-3</v>
       </c>
     </row>
     <row r="26" spans="1:14">
       <c r="A26" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B26">
-        <v>0.29781630003300003</v>
+        <v>0.52505835622499997</v>
       </c>
       <c r="C26">
-        <v>4.0449302027199999E-2</v>
+        <v>0.203099457451</v>
       </c>
       <c r="D26">
-        <v>1.5681822219E-2</v>
+        <v>4.1889420429199999E-2</v>
       </c>
       <c r="E26">
-        <v>4.2234778767100004E-3</v>
+        <v>1.5209091656499999E-2</v>
       </c>
       <c r="F26">
-        <v>0.37980985038699999</v>
+        <v>1.0660462077599999</v>
       </c>
       <c r="G26">
-        <v>7.6775131166400001E-2</v>
+        <v>0.34761333214899998</v>
       </c>
       <c r="H26">
-        <v>7.1728204485400002E-2</v>
+        <v>6.6610230671200005E-2</v>
       </c>
       <c r="I26">
-        <v>1.22806837352E-2</v>
+        <v>3.01488679722E-2</v>
       </c>
       <c r="J26">
-        <v>5.2453292880499998E-2</v>
+        <v>7.6770111947700004E-2</v>
       </c>
       <c r="K26">
-        <v>7.6377590244500002E-3</v>
+        <v>1.92107365818E-2</v>
       </c>
       <c r="L26">
-        <v>0.189595990435</v>
+        <v>7.9739633524500003E-2</v>
       </c>
       <c r="M26">
-        <v>3.2095626702099998E-2</v>
+        <v>5.90450283263E-2</v>
       </c>
       <c r="N26">
-        <v>3.8547348725099999E-3</v>
+        <v>5.5548225831700002E-3</v>
       </c>
     </row>
     <row r="27" spans="1:14">
       <c r="A27" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B27">
-        <v>0.42154485009600001</v>
+        <v>0.258725133863</v>
       </c>
       <c r="C27">
-        <v>0.22025467257199999</v>
+        <v>6.7428554688099995E-2</v>
       </c>
       <c r="D27">
-        <v>5.5069795328300003E-2</v>
+        <v>1.4605427421400001E-2</v>
       </c>
       <c r="E27">
-        <v>4.2559313626299999E-2</v>
+        <v>4.1079932917400001E-3</v>
       </c>
       <c r="F27">
-        <v>0.24085862439799999</v>
+        <v>0.20923454253400001</v>
       </c>
       <c r="G27">
-        <v>3.92509252837E-2</v>
+        <v>1.39381708609E-2</v>
       </c>
       <c r="H27">
-        <v>7.4110582985800005E-2</v>
+        <v>0.110383327874</v>
       </c>
       <c r="I27">
-        <v>1.6007382192299999E-2</v>
+        <v>7.1051986416099999E-2</v>
       </c>
       <c r="J27">
-        <v>0.111612573944</v>
+        <v>5.9892764184699999E-2</v>
       </c>
       <c r="K27">
-        <v>3.6013227203299997E-2</v>
+        <v>2.19465425924E-2</v>
       </c>
       <c r="L27">
-        <v>0.34027516914700001</v>
+        <v>0.56685422565700005</v>
       </c>
       <c r="M27">
-        <v>0.136348401614</v>
+        <v>0.44786850474000001</v>
       </c>
       <c r="N27">
-        <v>8.6278313539199999E-3</v>
+        <v>8.0895008298000008E-3</v>
       </c>
     </row>
     <row r="28" spans="1:14">
       <c r="A28" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B28">
-        <v>0.52505835622499997</v>
+        <v>1.3884252663000001</v>
       </c>
       <c r="C28">
-        <v>0.203099457451</v>
+        <v>0.35205241770399998</v>
       </c>
       <c r="D28">
-        <v>4.1889420429199999E-2</v>
+        <v>1.08554699152</v>
       </c>
       <c r="E28">
-        <v>1.5209091656499999E-2</v>
+        <v>0.29915157366900003</v>
       </c>
       <c r="F28">
-        <v>1.0660462077599999</v>
+        <v>0.51084091556</v>
       </c>
       <c r="G28">
-        <v>0.34761333214899998</v>
+        <v>9.5090435744100005E-2</v>
       </c>
       <c r="H28">
-        <v>6.6610230671200005E-2</v>
+        <v>0.63903576306599996</v>
       </c>
       <c r="I28">
-        <v>3.01488679722E-2</v>
+        <v>0.11992136502</v>
       </c>
       <c r="J28">
-        <v>7.6770111947700004E-2</v>
+        <v>0.78315507001700002</v>
       </c>
       <c r="K28">
-        <v>1.92107365818E-2</v>
+        <v>1.2837851057400001E-2</v>
       </c>
       <c r="L28">
-        <v>7.9739633524500003E-2</v>
+        <v>1.26389396708</v>
       </c>
       <c r="M28">
-        <v>5.90450283263E-2</v>
+        <v>0.147131078798</v>
       </c>
       <c r="N28">
-        <v>5.5548225831700002E-3</v>
+        <v>0.50022815021900002</v>
       </c>
     </row>
     <row r="29" spans="1:14">
       <c r="A29" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B29">
-        <v>0.258725133863</v>
+        <v>0.72557788985799998</v>
       </c>
       <c r="C29">
-        <v>6.7428554688099995E-2</v>
+        <v>0.110823963779</v>
       </c>
       <c r="D29">
-        <v>1.4605427421400001E-2</v>
+        <v>5.3074293896700001E-2</v>
       </c>
       <c r="E29">
-        <v>4.1079932917400001E-3</v>
+        <v>1.9599539011700001E-2</v>
       </c>
       <c r="F29">
-        <v>0.20923454253400001</v>
+        <v>0.73774549444399995</v>
       </c>
       <c r="G29">
-        <v>1.39381708609E-2</v>
+        <v>0.245500577507</v>
       </c>
       <c r="H29">
-        <v>0.110383327874</v>
+        <v>8.9961802756599998E-2</v>
       </c>
       <c r="I29">
-        <v>7.1051986416099999E-2</v>
+        <v>3.1252826897700002E-2</v>
       </c>
       <c r="J29">
-        <v>5.9892764184699999E-2</v>
+        <v>7.1611651001999996E-2</v>
       </c>
       <c r="K29">
-        <v>2.19465425924E-2</v>
+        <v>1.9215167349999999E-2</v>
       </c>
       <c r="L29">
-        <v>0.56685422565700005</v>
+        <v>0.129759296596</v>
       </c>
       <c r="M29">
-        <v>0.44786850474000001</v>
+        <v>5.25012810562E-2</v>
       </c>
       <c r="N29">
-        <v>8.0895008298000008E-3</v>
+        <v>6.9102293329299999E-3</v>
       </c>
     </row>
     <row r="30" spans="1:14">
       <c r="A30" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B30">
-        <v>1.3884252663000001</v>
+        <v>0.73384360491400003</v>
       </c>
       <c r="C30">
-        <v>0.35205241770399998</v>
+        <v>0.13872047463000001</v>
       </c>
       <c r="D30">
-        <v>1.08554699152</v>
+        <v>3.3785143390900003E-2</v>
       </c>
       <c r="E30">
-        <v>0.29915157366900003</v>
+        <v>7.6881185402999999E-3</v>
       </c>
       <c r="F30">
-        <v>0.51084091556</v>
+        <v>0.44311041349399999</v>
       </c>
       <c r="G30">
-        <v>9.5090435744100005E-2</v>
+        <v>7.1899266577899995E-2</v>
       </c>
       <c r="H30">
-        <v>0.63903576306599996</v>
+        <v>4.7951273195599997E-2</v>
       </c>
       <c r="I30">
-        <v>0.11992136502</v>
+        <v>2.3115070260800001E-2</v>
       </c>
       <c r="J30">
-        <v>0.78315507001700002</v>
+        <v>4.6594141080500001E-2</v>
       </c>
       <c r="K30">
-        <v>1.2837851057400001E-2</v>
+        <v>1.14338847228E-2</v>
       </c>
       <c r="L30">
-        <v>1.26389396708</v>
+        <v>0.11469395938800001</v>
       </c>
       <c r="M30">
-        <v>0.147131078798</v>
+        <v>5.3741323932799998E-2</v>
       </c>
       <c r="N30">
-        <v>0.50022815021900002</v>
+        <v>2.49331397856E-3</v>
       </c>
     </row>
     <row r="31" spans="1:14">
       <c r="A31" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B31">
-        <v>0.72557788985799998</v>
+        <v>0.76993803703599994</v>
       </c>
       <c r="C31">
-        <v>0.110823963779</v>
+        <v>0.21084435955799999</v>
       </c>
       <c r="D31">
-        <v>5.3074293896700001E-2</v>
+        <v>2.6216326287900001E-2</v>
       </c>
       <c r="E31">
-        <v>1.9599539011700001E-2</v>
+        <v>1.17700229531E-2</v>
       </c>
       <c r="F31">
-        <v>0.73774549444399995</v>
+        <v>0.42048363184900001</v>
       </c>
       <c r="G31">
-        <v>0.245500577507</v>
+        <v>0.121411719696</v>
       </c>
       <c r="H31">
-        <v>8.9961802756599998E-2</v>
+        <v>2.6132134210100001E-2</v>
       </c>
       <c r="I31">
-        <v>3.1252826897700002E-2</v>
+        <v>7.1466218393300002E-3</v>
       </c>
       <c r="J31">
-        <v>7.1611651001999996E-2</v>
+        <v>3.3088500017399998E-2</v>
       </c>
       <c r="K31">
-        <v>1.9215167349999999E-2</v>
+        <v>1.1392567526399999E-2</v>
       </c>
       <c r="L31">
-        <v>0.129759296596</v>
+        <v>6.4234734211799996E-2</v>
       </c>
       <c r="M31">
-        <v>5.25012810562E-2</v>
+        <v>1.2459946674400001E-2</v>
       </c>
       <c r="N31">
-        <v>6.9102293329299999E-3</v>
+        <v>9.4570955368900001E-4</v>
       </c>
     </row>
     <row r="32" spans="1:14">
       <c r="A32" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B32">
-        <v>0.73384360491400003</v>
+        <v>0.84247514634800003</v>
       </c>
       <c r="C32">
-        <v>0.13872047463000001</v>
+        <v>0.119671772392</v>
       </c>
       <c r="D32">
-        <v>3.3785143390900003E-2</v>
+        <v>4.12776773822E-3</v>
       </c>
       <c r="E32">
-        <v>7.6881185402999999E-3</v>
+        <v>3.7770966217500002E-3</v>
       </c>
       <c r="F32">
-        <v>0.44311041349399999</v>
+        <v>0.200354582369</v>
       </c>
       <c r="G32">
-        <v>7.1899266577899995E-2</v>
+        <v>2.0286030423499999E-2</v>
       </c>
       <c r="H32">
-        <v>4.7951273195599997E-2</v>
+        <v>3.9580125228499997E-3</v>
       </c>
       <c r="I32">
-        <v>2.3115070260800001E-2</v>
+        <v>1.55426256924E-3</v>
       </c>
       <c r="J32">
-        <v>4.6594141080500001E-2</v>
+        <v>5.1241569750100002E-3</v>
       </c>
       <c r="K32">
-        <v>1.14338847228E-2</v>
+        <v>5.30307740488E-3</v>
       </c>
       <c r="L32">
-        <v>0.11469395938800001</v>
+        <v>2.07306030001E-2</v>
       </c>
       <c r="M32">
-        <v>5.3741323932799998E-2</v>
-      </c>
-      <c r="N32">
-        <v>2.49331397856E-3</v>
+        <v>7.8974010086700006E-3</v>
+      </c>
+      <c r="N32" s="1">
+        <v>1.22259882933E-5</v>
       </c>
     </row>
     <row r="33" spans="1:14">
       <c r="A33" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B33">
-        <v>0.76993803703599994</v>
+        <v>0.55258076338899997</v>
       </c>
       <c r="C33">
-        <v>0.21084435955799999</v>
+        <v>0.26220308905099998</v>
       </c>
       <c r="D33">
-        <v>2.6216326287900001E-2</v>
+        <v>2.97772172673E-3</v>
       </c>
       <c r="E33">
-        <v>1.17700229531E-2</v>
+        <v>1.2211526825400001E-3</v>
       </c>
       <c r="F33">
-        <v>0.42048363184900001</v>
+        <v>0.24972070823500001</v>
       </c>
       <c r="G33">
-        <v>0.121411719696</v>
+        <v>5.7026140056900002E-2</v>
       </c>
       <c r="H33">
-        <v>2.6132134210100001E-2</v>
+        <v>1.1004656193500001E-2</v>
       </c>
       <c r="I33">
-        <v>7.1466218393300002E-3</v>
+        <v>2.1290164135400001E-3</v>
       </c>
       <c r="J33">
-        <v>3.3088500017399998E-2</v>
+        <v>5.7205839806699996E-3</v>
       </c>
       <c r="K33">
-        <v>1.1392567526399999E-2</v>
+        <v>8.2598420851600002E-4</v>
       </c>
       <c r="L33">
-        <v>6.4234734211799996E-2</v>
+        <v>4.9154354770999997E-2</v>
       </c>
       <c r="M33">
-        <v>1.2459946674400001E-2</v>
-      </c>
-      <c r="N33">
-        <v>9.4570955368900001E-4</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14">
-      <c r="A34" t="s">
-        <v>46</v>
-      </c>
-      <c r="B34">
-        <v>0.84247514634800003</v>
-      </c>
-      <c r="C34">
-        <v>0.119671772392</v>
-      </c>
-      <c r="D34">
-        <v>4.12776773822E-3</v>
-      </c>
-      <c r="E34">
-        <v>3.7770966217500002E-3</v>
-      </c>
-      <c r="F34">
-        <v>0.200354582369</v>
-      </c>
-      <c r="G34">
-        <v>2.0286030423499999E-2</v>
-      </c>
-      <c r="H34">
-        <v>3.9580125228499997E-3</v>
-      </c>
-      <c r="I34">
-        <v>1.55426256924E-3</v>
-      </c>
-      <c r="J34">
-        <v>5.1241569750100002E-3</v>
-      </c>
-      <c r="K34">
-        <v>5.30307740488E-3</v>
-      </c>
-      <c r="L34">
-        <v>2.07306030001E-2</v>
-      </c>
-      <c r="M34">
-        <v>7.8974010086700006E-3</v>
-      </c>
-      <c r="N34" s="1">
-        <v>1.22259882933E-5</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14">
-      <c r="A35" t="s">
-        <v>47</v>
-      </c>
-      <c r="B35">
-        <v>0.55258076338899997</v>
-      </c>
-      <c r="C35">
-        <v>0.26220308905099998</v>
-      </c>
-      <c r="D35">
-        <v>2.97772172673E-3</v>
-      </c>
-      <c r="E35">
-        <v>1.2211526825400001E-3</v>
-      </c>
-      <c r="F35">
-        <v>0.24972070823500001</v>
-      </c>
-      <c r="G35">
-        <v>5.7026140056900002E-2</v>
-      </c>
-      <c r="H35">
-        <v>1.1004656193500001E-2</v>
-      </c>
-      <c r="I35">
-        <v>2.1290164135400001E-3</v>
-      </c>
-      <c r="J35">
-        <v>5.7205839806699996E-3</v>
-      </c>
-      <c r="K35">
-        <v>8.2598420851600002E-4</v>
-      </c>
-      <c r="L35">
-        <v>4.9154354770999997E-2</v>
-      </c>
-      <c r="M35">
         <v>2.2006027600200002E-2</v>
       </c>
-      <c r="N35" s="1">
+      <c r="N33" s="1">
         <v>6.4645845540200006E-5</v>
       </c>
     </row>

</xml_diff>